<commit_message>
Completed basic implementation for the requestForm service of the KnowledgeBase. One test still being finessed
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -7,14 +7,21 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Manifest" sheetId="1" r:id="rId1"/>
+    <sheet name="Posting Label" sheetId="1" r:id="rId1"/>
+    <sheet name="Manifest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>In test_as_excel.py</t>
+  </si>
   <si>
     <t>UID</t>
   </si>
@@ -561,9 +568,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -580,60 +613,60 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -645,39 +678,39 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -689,10 +722,10 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -704,10 +737,10 @@
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -717,16 +750,16 @@
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -738,10 +771,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -753,10 +786,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -766,16 +799,16 @@
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -787,10 +820,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -802,10 +835,10 @@
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
       <c r="H12" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -815,16 +848,16 @@
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -836,10 +869,10 @@
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -851,10 +884,10 @@
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -864,16 +897,16 @@
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -885,10 +918,10 @@
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -900,10 +933,10 @@
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -911,10 +944,10 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
@@ -926,10 +959,10 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>

</xml_diff>

<commit_message>
Completed test for generating forms, including validating formats and layouts
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -15,12 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>In test_as_excel.py</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+  <si>
+    <t>Testing from</t>
+  </si>
+  <si>
+    <t>Verifying</t>
+  </si>
+  <si>
+    <t>test_as_excel.py</t>
+  </si>
+  <si>
+    <t>Correct population of Excel with respect to data, layout and formatting</t>
   </si>
   <si>
     <t>UID</t>
@@ -230,13 +236,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFE8E8E8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEBF1DE"/>
+        <fgColor rgb="FFE5EDD3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,12 +256,18 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -267,10 +279,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -568,14 +580,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C2"/>
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
@@ -583,7 +595,15 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -613,60 +633,60 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -678,39 +698,39 @@
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -722,10 +742,10 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -737,10 +757,10 @@
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -750,16 +770,16 @@
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -771,10 +791,10 @@
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -786,10 +806,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -799,16 +819,16 @@
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -820,10 +840,10 @@
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -835,10 +855,10 @@
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
       <c r="H12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -848,16 +868,16 @@
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -869,10 +889,10 @@
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
       <c r="H14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -884,10 +904,10 @@
       <c r="F15" s="2"/>
       <c r="G15" s="3"/>
       <c r="H15" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -897,16 +917,16 @@
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -918,10 +938,10 @@
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -933,10 +953,10 @@
       <c r="F18" s="2"/>
       <c r="G18" s="3"/>
       <c r="H18" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -944,10 +964,10 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
@@ -959,10 +979,10 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>

</xml_diff>

<commit_message>
Fixed an inadvertent problem with prior commit
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Testing from</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Correct population of Excel with respect to data, layout and formatting</t>
+  </si>
+  <si>
+    <t>Posting Label</t>
   </si>
   <si>
     <t>UID</t>
@@ -204,10 +207,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,9 +285,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -580,7 +592,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -590,19 +602,24 @@
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" spans="2:3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -632,362 +649,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="2" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="I6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="I10" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="I11" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>34</v>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="G13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>21</v>
+      <c r="H13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>23</v>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>34</v>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="G16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>21</v>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>34</v>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>34</v>
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
+      <c r="E19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
+      <c r="E20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0"/>

</xml_diff>

<commit_message>
Updated colors for generated forms
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -247,13 +247,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8E8E8"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE5EDD3"/>
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>

<commit_message>
Added data.kind, data.range, data.sheet to generatedForm's posting labels
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Testing from</t>
   </si>
@@ -23,10 +23,28 @@
     <t>Verifying</t>
   </si>
   <si>
+    <t>data.kind.57</t>
+  </si>
+  <si>
+    <t>data.range.57</t>
+  </si>
+  <si>
+    <t>data.sheet.57</t>
+  </si>
+  <si>
     <t>test_as_excel.py</t>
   </si>
   <si>
     <t>Correct population of Excel with respect to data, layout and formatting</t>
+  </si>
+  <si>
+    <t>Manifest for test_dataframe_2_xl</t>
+  </si>
+  <si>
+    <t>A1:I20</t>
+  </si>
+  <si>
+    <t>Manifest</t>
   </si>
   <si>
     <t>Posting Label</t>
@@ -592,19 +610,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C3"/>
+  <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:3">
@@ -612,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3">
@@ -620,7 +638,31 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -650,60 +692,60 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -715,39 +757,39 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -759,10 +801,10 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -774,10 +816,10 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -787,16 +829,16 @@
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -808,10 +850,10 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -823,10 +865,10 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -836,16 +878,16 @@
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -857,10 +899,10 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -872,10 +914,10 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -885,16 +927,16 @@
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -906,10 +948,10 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -921,10 +963,10 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -934,16 +976,16 @@
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -955,10 +997,10 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -970,10 +1012,10 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -981,10 +1023,10 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
@@ -996,10 +1038,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>

</xml_diff>

<commit_message>
Fixed formatting issues with generated forms
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -616,8 +616,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
@@ -679,15 +679,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>

<commit_message>
Prepared generatedForms for upcoming update functionality by adding version and formulas
</commit_message>
<xml_diff>
--- a/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
+++ b/src/apodeixi/representers/tests_unit/output_data/test_dataframe_2_xl_MANIFEST.xlsx
@@ -80,145 +80,145 @@
     <t>JTBD1</t>
   </si>
   <si>
+    <t>JTBD2</t>
+  </si>
+  <si>
     <t>Quickly add features to Apodeixi</t>
   </si>
   <si>
+    <t>Transform the products</t>
+  </si>
+  <si>
     <t>Apodeixi developers</t>
   </si>
   <si>
+    <t>Product teams, architects</t>
+  </si>
+  <si>
     <t>JTBD1.C1</t>
   </si>
   <si>
+    <t>JTBD2.C1</t>
+  </si>
+  <si>
+    <t>JTBD2.C2</t>
+  </si>
+  <si>
+    <t>JTBD2.C3</t>
+  </si>
+  <si>
     <t>Scaffolding for BDD tests</t>
   </si>
   <si>
+    <t>Create roadmap</t>
+  </si>
+  <si>
+    <t>Stress-test roadmap</t>
+  </si>
+  <si>
+    <t>Back-test roadmap</t>
+  </si>
+  <si>
     <t>JTBD1.C1.F1</t>
   </si>
   <si>
+    <t>JTBD2.C1.F1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F3</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F4</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F5</t>
+  </si>
+  <si>
     <t>Drive scaffolding from Apodeixi capability documentation</t>
   </si>
   <si>
+    <t>Define big rocks</t>
+  </si>
+  <si>
+    <t>Define milestones</t>
+  </si>
+  <si>
+    <t>Import epics</t>
+  </si>
+  <si>
+    <t>Epics mapping</t>
+  </si>
+  <si>
+    <t>Compute roadmap</t>
+  </si>
+  <si>
     <t>JTBD1.C1.F1.S1</t>
   </si>
   <si>
+    <t>JTBD1.C1.F1.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F1.S1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F1.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F1.S3</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F2.S1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F2.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F2.S3</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F3.S1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F3.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F3.S3</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F4.S1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F4.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F4.S3</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F5.S1</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F5.S2</t>
+  </si>
+  <si>
+    <t>JTBD2.C1.F5.S3</t>
+  </si>
+  <si>
     <t>Create</t>
   </si>
   <si>
-    <t>JTBD1.C1.F1.S2</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
-    <t>JTBD2</t>
-  </si>
-  <si>
-    <t>Transform the products</t>
-  </si>
-  <si>
-    <t>Product teams, architects</t>
-  </si>
-  <si>
-    <t>JTBD2.C1</t>
-  </si>
-  <si>
-    <t>Create roadmap</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F1</t>
-  </si>
-  <si>
-    <t>Define big rocks</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F1.S1</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F1.S2</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F1.S3</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
-    <t>JTBD2.C1.F2</t>
-  </si>
-  <si>
-    <t>Define milestones</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F2.S1</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F2.S2</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F2.S3</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F3</t>
-  </si>
-  <si>
-    <t>Import epics</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F3.S1</t>
-  </si>
-  <si>
     <t>First import</t>
   </si>
   <si>
-    <t>JTBD2.C1.F3.S2</t>
-  </si>
-  <si>
     <t>Refresh imports</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F3.S3</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F4</t>
-  </si>
-  <si>
-    <t>Epics mapping</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F4.S1</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F4.S2</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F4.S3</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F5</t>
-  </si>
-  <si>
-    <t>Compute roadmap</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F5.S1</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F5.S2</t>
-  </si>
-  <si>
-    <t>JTBD2.C1.F5.S3</t>
-  </si>
-  <si>
-    <t>JTBD2.C2</t>
-  </si>
-  <si>
-    <t>Stress-test roadmap</t>
-  </si>
-  <si>
-    <t>JTBD2.C3</t>
-  </si>
-  <si>
-    <t>Back-test roadmap</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -724,28 +724,28 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -757,39 +757,39 @@
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -801,10 +801,10 @@
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -816,10 +816,10 @@
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -829,16 +829,16 @@
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -850,10 +850,10 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -865,10 +865,10 @@
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -878,16 +878,16 @@
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -899,10 +899,10 @@
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -914,10 +914,10 @@
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -927,16 +927,16 @@
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -948,10 +948,10 @@
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -963,10 +963,10 @@
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -976,16 +976,16 @@
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="I16" s="4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -997,10 +997,10 @@
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1012,10 +1012,10 @@
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1023,10 +1023,10 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
@@ -1038,10 +1038,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>

</xml_diff>